<commit_message>
Tabla costo hamming 1
</commit_message>
<xml_diff>
--- a/PruebasTaller2.xlsx
+++ b/PruebasTaller2.xlsx
@@ -1934,7 +1934,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F76"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2287,15 +2287,11 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>111</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
+      <c r="A14" t="n">
+        <v>111</v>
+      </c>
+      <c r="B14" t="n">
+        <v>100</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
@@ -2312,6 +2308,1622 @@
         <is>
           <t xml:space="preserve">⎛ A ⎞⎛  ∅  ⎞
 ⎝ ∅ ⎠⎝ b,c ⎠
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>111</v>
+      </c>
+      <c r="B15" t="n">
+        <v>100</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Geometric</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>1</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.009550809860229492</v>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">⎛ A ⎞⎛  ∅  ⎞
+⎝ ∅ ⎠⎝ b,c ⎠
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>111</v>
+      </c>
+      <c r="B16" t="n">
+        <v>100</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Geometric</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>1</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.004679441452026367</v>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t xml:space="preserve">⎛ A ⎞⎛  ∅  ⎞
+⎝ ∅ ⎠⎝ b,c ⎠
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>111</v>
+      </c>
+      <c r="B17" t="n">
+        <v>100</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Geometric</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>1</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0.01165103912353516</v>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t xml:space="preserve">⎛ A ⎞⎛  ∅  ⎞
+⎝ ∅ ⎠⎝ b,c ⎠
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>111</v>
+      </c>
+      <c r="B18" t="n">
+        <v>100</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Geometric</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>1</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0.01384067535400391</v>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t xml:space="preserve">⎛ A ⎞⎛  ∅  ⎞
+⎝ ∅ ⎠⎝ b,c ⎠
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>111</v>
+      </c>
+      <c r="B19" t="n">
+        <v>100</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Geometric</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>1</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0.01005959510803223</v>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">⎛ A ⎞⎛  ∅  ⎞
+⎝ ∅ ⎠⎝ b,c ⎠
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>111</v>
+      </c>
+      <c r="B20" t="n">
+        <v>100</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Geometric</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>1</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0.01100063323974609</v>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t xml:space="preserve">⎛ A ⎞⎛  ∅  ⎞
+⎝ ∅ ⎠⎝ b,c ⎠
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>111</v>
+      </c>
+      <c r="B21" t="n">
+        <v>100</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Geometric</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>1</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0.009033441543579102</v>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t xml:space="preserve">⎛ A ⎞⎛  ∅  ⎞
+⎝ ∅ ⎠⎝ b,c ⎠
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>111</v>
+      </c>
+      <c r="B22" t="n">
+        <v>100</v>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Geometric</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>1</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0.01900601387023926</v>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t xml:space="preserve">⎛ A ⎞⎛  ∅  ⎞
+⎝ ∅ ⎠⎝ b,c ⎠
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>111</v>
+      </c>
+      <c r="B23" t="n">
+        <v>100</v>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Geometric</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>1</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0.01064467430114746</v>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t xml:space="preserve">⎛ A ⎞⎛  ∅  ⎞
+⎝ ∅ ⎠⎝ b,c ⎠
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>111</v>
+      </c>
+      <c r="B24" t="n">
+        <v>100</v>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Geometric</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>1</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0.009000301361083984</v>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t xml:space="preserve">⎛ A ⎞⎛  ∅  ⎞
+⎝ ∅ ⎠⎝ b,c ⎠
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>111</v>
+      </c>
+      <c r="B25" t="n">
+        <v>100</v>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Geometric</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>1</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0.009794473648071289</v>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t xml:space="preserve">⎛ A ⎞⎛  ∅  ⎞
+⎝ ∅ ⎠⎝ b,c ⎠
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>111</v>
+      </c>
+      <c r="B26" t="n">
+        <v>100</v>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Geometric</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>1</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0.00892329216003418</v>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t xml:space="preserve">⎛ A ⎞⎛  ∅  ⎞
+⎝ ∅ ⎠⎝ b,c ⎠
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>111</v>
+      </c>
+      <c r="B27" t="n">
+        <v>100</v>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Geometric</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>1</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0.01892924308776855</v>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t xml:space="preserve">⎛ A ⎞⎛  ∅  ⎞
+⎝ ∅ ⎠⎝ b,c ⎠
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>111</v>
+      </c>
+      <c r="B28" t="n">
+        <v>100</v>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Geometric</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>1</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0.02087903022766113</v>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t xml:space="preserve">⎛ A ⎞⎛  ∅  ⎞
+⎝ ∅ ⎠⎝ b,c ⎠
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>111</v>
+      </c>
+      <c r="B29" t="n">
+        <v>100</v>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Geometric</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>1</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0.01861906051635742</v>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t xml:space="preserve">⎛ A ⎞⎛  ∅  ⎞
+⎝ ∅ ⎠⎝ b,c ⎠
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>111</v>
+      </c>
+      <c r="B30" t="n">
+        <v>100</v>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Geometric</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>1</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0.01829314231872559</v>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t xml:space="preserve">⎛ A ⎞⎛  ∅  ⎞
+⎝ ∅ ⎠⎝ b,c ⎠
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>111</v>
+      </c>
+      <c r="B31" t="n">
+        <v>100</v>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Geometric</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>1</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0.01772165298461914</v>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t xml:space="preserve">⎛ A ⎞⎛  ∅  ⎞
+⎝ ∅ ⎠⎝ b,c ⎠
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>111</v>
+      </c>
+      <c r="B32" t="n">
+        <v>100</v>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Geometric</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>1</v>
+      </c>
+      <c r="E32" t="n">
+        <v>0.01593661308288574</v>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t xml:space="preserve">⎛ A ⎞⎛  ∅  ⎞
+⎝ ∅ ⎠⎝ b,c ⎠
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>111</v>
+      </c>
+      <c r="B33" t="n">
+        <v>100</v>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Geometric</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>1</v>
+      </c>
+      <c r="E33" t="n">
+        <v>0.02242517471313477</v>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t xml:space="preserve">⎛ A ⎞⎛  ∅  ⎞
+⎝ ∅ ⎠⎝ b,c ⎠
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>111</v>
+      </c>
+      <c r="B34" t="n">
+        <v>100</v>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Geometric</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>1</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0.009336233139038086</v>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t xml:space="preserve">⎛ A ⎞⎛  ∅  ⎞
+⎝ ∅ ⎠⎝ b,c ⎠
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>111</v>
+      </c>
+      <c r="B35" t="n">
+        <v>100</v>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Geometric</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>1</v>
+      </c>
+      <c r="E35" t="n">
+        <v>0.00996708869934082</v>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t xml:space="preserve">⎛ A ⎞⎛  ∅  ⎞
+⎝ ∅ ⎠⎝ b,c ⎠
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>111</v>
+      </c>
+      <c r="B36" t="n">
+        <v>100</v>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Geometric</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>1</v>
+      </c>
+      <c r="E36" t="n">
+        <v>0.0143890380859375</v>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t xml:space="preserve">⎛ A ⎞⎛  ∅  ⎞
+⎝ ∅ ⎠⎝ b,c ⎠
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>111</v>
+      </c>
+      <c r="B37" t="n">
+        <v>100</v>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Geometric</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>1</v>
+      </c>
+      <c r="E37" t="n">
+        <v>0.008543729782104492</v>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t xml:space="preserve">⎛ A ⎞⎛  ∅  ⎞
+⎝ ∅ ⎠⎝ b,c ⎠
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>111</v>
+      </c>
+      <c r="B38" t="n">
+        <v>100</v>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Geometric</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>1</v>
+      </c>
+      <c r="E38" t="n">
+        <v>0.01018834114074707</v>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t xml:space="preserve">⎛ A ⎞⎛  ∅  ⎞
+⎝ ∅ ⎠⎝ b,c ⎠
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>111</v>
+      </c>
+      <c r="B39" t="n">
+        <v>100</v>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Geometric</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>1</v>
+      </c>
+      <c r="E39" t="n">
+        <v>0.008052825927734375</v>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t xml:space="preserve">⎛ A ⎞⎛  ∅  ⎞
+⎝ ∅ ⎠⎝ b,c ⎠
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>111</v>
+      </c>
+      <c r="B40" t="n">
+        <v>100</v>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Geometric</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>1</v>
+      </c>
+      <c r="E40" t="n">
+        <v>0.01607632637023926</v>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t xml:space="preserve">⎛ A ⎞⎛  ∅  ⎞
+⎝ ∅ ⎠⎝ b,c ⎠
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>111</v>
+      </c>
+      <c r="B41" t="n">
+        <v>100</v>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Geometric</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>1</v>
+      </c>
+      <c r="E41" t="n">
+        <v>0.02606368064880371</v>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t xml:space="preserve">⎛ A ⎞⎛  ∅  ⎞
+⎝ ∅ ⎠⎝ b,c ⎠
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>111</v>
+      </c>
+      <c r="B42" t="n">
+        <v>100</v>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Geometric</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>1</v>
+      </c>
+      <c r="E42" t="n">
+        <v>0.00594639778137207</v>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t xml:space="preserve">⎛ A ⎞⎛  ∅  ⎞
+⎝ ∅ ⎠⎝ b,c ⎠
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>111</v>
+      </c>
+      <c r="B43" t="n">
+        <v>100</v>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Geometric</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>1</v>
+      </c>
+      <c r="E43" t="n">
+        <v>0.01153802871704102</v>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t xml:space="preserve">⎛ A ⎞⎛  ∅  ⎞
+⎝ ∅ ⎠⎝ b,c ⎠
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>111</v>
+      </c>
+      <c r="B44" t="n">
+        <v>100</v>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Geometric</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>1</v>
+      </c>
+      <c r="E44" t="n">
+        <v>0.01173710823059082</v>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t xml:space="preserve">⎛ A ⎞⎛  ∅  ⎞
+⎝ ∅ ⎠⎝ b,c ⎠
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>111</v>
+      </c>
+      <c r="B45" t="n">
+        <v>100</v>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Geometric</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>1</v>
+      </c>
+      <c r="E45" t="n">
+        <v>0.006221771240234375</v>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t xml:space="preserve">⎛ A ⎞⎛  ∅  ⎞
+⎝ ∅ ⎠⎝ b,c ⎠
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>111</v>
+      </c>
+      <c r="B46" t="n">
+        <v>100</v>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Geometric</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>1</v>
+      </c>
+      <c r="E46" t="n">
+        <v>0.005696296691894531</v>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t xml:space="preserve">⎛ A ⎞⎛  ∅  ⎞
+⎝ ∅ ⎠⎝ b,c ⎠
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>111</v>
+      </c>
+      <c r="B47" t="n">
+        <v>100</v>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Geometric</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>1</v>
+      </c>
+      <c r="E47" t="n">
+        <v>0.006389617919921875</v>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t xml:space="preserve">⎛ A ⎞⎛  ∅  ⎞
+⎝ ∅ ⎠⎝ b,c ⎠
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>111</v>
+      </c>
+      <c r="B48" t="n">
+        <v>111</v>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Geometric</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="E48" t="n">
+        <v>0.006340742111206055</v>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t xml:space="preserve">⎛ A ⎞⎛  ∅  ⎞
+⎝ ∅ ⎠⎝ b,c ⎠
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>111</v>
+      </c>
+      <c r="B49" t="n">
+        <v>110</v>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Geometric</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>1</v>
+      </c>
+      <c r="E49" t="n">
+        <v>0.008653163909912109</v>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t xml:space="preserve">⎛ A ⎞⎛  ∅  ⎞
+⎝ ∅ ⎠⎝ b,c ⎠
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>111</v>
+      </c>
+      <c r="B50" t="n">
+        <v>101</v>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Geometric</t>
+        </is>
+      </c>
+      <c r="D50" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="E50" t="n">
+        <v>0.01100611686706543</v>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t xml:space="preserve">⎛ A ⎞⎛  ∅  ⎞
+⎝ ∅ ⎠⎝ b,c ⎠
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>111</v>
+      </c>
+      <c r="B51" t="n">
+        <v>100</v>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Geometric</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>1</v>
+      </c>
+      <c r="E51" t="n">
+        <v>0.00433039665222168</v>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t xml:space="preserve">⎛ A ⎞⎛  ∅  ⎞
+⎝ ∅ ⎠⎝ b,c ⎠
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>111</v>
+      </c>
+      <c r="B52" t="n">
+        <v>100</v>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Geometric</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>1</v>
+      </c>
+      <c r="E52" t="n">
+        <v>0.005023956298828125</v>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t xml:space="preserve">⎛ A ⎞⎛  ∅  ⎞
+⎝ ∅ ⎠⎝ b,c ⎠
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>111</v>
+      </c>
+      <c r="B53" t="n">
+        <v>100</v>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Geometric</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>1</v>
+      </c>
+      <c r="E53" t="n">
+        <v>0.005236625671386719</v>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t xml:space="preserve">⎛ A ⎞⎛  ∅  ⎞
+⎝ ∅ ⎠⎝ b,c ⎠
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>111</v>
+      </c>
+      <c r="B54" t="n">
+        <v>100</v>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Geometric</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>1</v>
+      </c>
+      <c r="E54" t="n">
+        <v>0.003515958786010742</v>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t xml:space="preserve">⎛ A ⎞⎛  ∅  ⎞
+⎝ ∅ ⎠⎝ b,c ⎠
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>111</v>
+      </c>
+      <c r="B55" t="n">
+        <v>100</v>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Geometric</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>1</v>
+      </c>
+      <c r="E55" t="n">
+        <v>0.007149219512939453</v>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t xml:space="preserve">⎛ A ⎞⎛  ∅  ⎞
+⎝ ∅ ⎠⎝ b,c ⎠
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>111</v>
+      </c>
+      <c r="B56" t="n">
+        <v>100</v>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Geometric</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>1</v>
+      </c>
+      <c r="E56" t="n">
+        <v>0.006177186965942383</v>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t xml:space="preserve">⎛ A ⎞⎛  ∅  ⎞
+⎝ ∅ ⎠⎝ b,c ⎠
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>111</v>
+      </c>
+      <c r="B57" t="n">
+        <v>110</v>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Geometric</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>1</v>
+      </c>
+      <c r="E57" t="n">
+        <v>0.004501819610595703</v>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t xml:space="preserve">⎛ A ⎞⎛  ∅  ⎞
+⎝ ∅ ⎠⎝ b,c ⎠
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>111</v>
+      </c>
+      <c r="B58" t="n">
+        <v>110</v>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Geometric</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>1</v>
+      </c>
+      <c r="E58" t="n">
+        <v>0.004956722259521484</v>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t xml:space="preserve">⎛ A ⎞⎛  ∅  ⎞
+⎝ ∅ ⎠⎝ b,c ⎠
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>111</v>
+      </c>
+      <c r="B59" t="n">
+        <v>11</v>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Geometric</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="E59" t="n">
+        <v>0.006601095199584961</v>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t xml:space="preserve">⎛ B ⎞⎛  ∅  ⎞
+⎝ ∅ ⎠⎝ a,c ⎠
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>111</v>
+      </c>
+      <c r="B60" t="n">
+        <v>11</v>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Geometric</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="E60" t="n">
+        <v>0.007421970367431641</v>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t xml:space="preserve">⎛ B ⎞⎛  ∅  ⎞
+⎝ ∅ ⎠⎝ a,c ⎠
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>111</v>
+      </c>
+      <c r="B61" t="n">
+        <v>11</v>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Geometric</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="E61" t="n">
+        <v>0.006676673889160156</v>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t xml:space="preserve">⎛ B ⎞⎛  ∅  ⎞
+⎝ ∅ ⎠⎝ a,c ⎠
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>111</v>
+      </c>
+      <c r="B62" t="n">
+        <v>11</v>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Geometric</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="E62" t="n">
+        <v>0.008481264114379883</v>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t xml:space="preserve">⎛ B ⎞⎛  ∅  ⎞
+⎝ ∅ ⎠⎝ a,c ⎠
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>111</v>
+      </c>
+      <c r="B63" t="n">
+        <v>11</v>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Geometric</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="E63" t="n">
+        <v>0.005858898162841797</v>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t xml:space="preserve">⎛ B ⎞⎛  ∅  ⎞
+⎝ ∅ ⎠⎝ a,c ⎠
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>111</v>
+      </c>
+      <c r="B64" t="n">
+        <v>11</v>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Geometric</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="E64" t="n">
+        <v>0.006037473678588867</v>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t xml:space="preserve">⎛ B ⎞⎛  ∅  ⎞
+⎝ ∅ ⎠⎝ a,c ⎠
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>111</v>
+      </c>
+      <c r="B65" t="n">
+        <v>11</v>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Geometric</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="E65" t="n">
+        <v>0.005830049514770508</v>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t xml:space="preserve">⎛ B ⎞⎛  ∅  ⎞
+⎝ ∅ ⎠⎝ a,c ⎠
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>111</v>
+      </c>
+      <c r="B66" t="n">
+        <v>11</v>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Geometric</t>
+        </is>
+      </c>
+      <c r="D66" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="E66" t="n">
+        <v>0.005349159240722656</v>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t xml:space="preserve">⎛ B ⎞⎛  ∅  ⎞
+⎝ ∅ ⎠⎝ a,c ⎠
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>111</v>
+      </c>
+      <c r="B67" t="n">
+        <v>110</v>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Geometric</t>
+        </is>
+      </c>
+      <c r="D67" t="n">
+        <v>1</v>
+      </c>
+      <c r="E67" t="n">
+        <v>0.005518436431884766</v>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t xml:space="preserve">⎛ A ⎞⎛  ∅  ⎞
+⎝ ∅ ⎠⎝ b,c ⎠
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>111</v>
+      </c>
+      <c r="B68" t="n">
+        <v>11</v>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>Geometric</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="E68" t="n">
+        <v>0.005942106246948242</v>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t xml:space="preserve">⎛ B ⎞⎛  ∅  ⎞
+⎝ ∅ ⎠⎝ a,c ⎠
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>111</v>
+      </c>
+      <c r="B69" t="n">
+        <v>101</v>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>Geometric</t>
+        </is>
+      </c>
+      <c r="D69" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="E69" t="n">
+        <v>0.005138635635375977</v>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t xml:space="preserve">⎛ A ⎞⎛  ∅  ⎞
+⎝ ∅ ⎠⎝ b,c ⎠
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>111</v>
+      </c>
+      <c r="B70" t="n">
+        <v>11</v>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>Geometric</t>
+        </is>
+      </c>
+      <c r="D70" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="E70" t="n">
+        <v>0.005536317825317383</v>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t xml:space="preserve">⎛ B ⎞⎛  ∅  ⎞
+⎝ ∅ ⎠⎝ a,c ⎠
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>111</v>
+      </c>
+      <c r="B71" t="n">
+        <v>101</v>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>Geometric</t>
+        </is>
+      </c>
+      <c r="D71" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="E71" t="n">
+        <v>0.005004405975341797</v>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t xml:space="preserve">⎛ A ⎞⎛  ∅  ⎞
+⎝ ∅ ⎠⎝ b,c ⎠
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>111</v>
+      </c>
+      <c r="B72" t="n">
+        <v>101</v>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>Geometric</t>
+        </is>
+      </c>
+      <c r="D72" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="E72" t="n">
+        <v>0.005203008651733398</v>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t xml:space="preserve">⎛ A ⎞⎛  ∅  ⎞
+⎝ ∅ ⎠⎝ b,c ⎠
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>111</v>
+      </c>
+      <c r="B73" t="n">
+        <v>101</v>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>Geometric</t>
+        </is>
+      </c>
+      <c r="D73" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="E73" t="n">
+        <v>0.005002021789550781</v>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t xml:space="preserve">⎛ A ⎞⎛  ∅  ⎞
+⎝ ∅ ⎠⎝ b,c ⎠
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>111</v>
+      </c>
+      <c r="B74" t="n">
+        <v>11</v>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Geometric</t>
+        </is>
+      </c>
+      <c r="D74" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="E74" t="n">
+        <v>0.005002021789550781</v>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t xml:space="preserve">⎛ B ⎞⎛  ∅  ⎞
+⎝ ∅ ⎠⎝ a,c ⎠
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>11111</v>
+      </c>
+      <c r="B75" t="n">
+        <v>111111</v>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>Geometric</t>
+        </is>
+      </c>
+      <c r="D75" t="n">
+        <v>2.3125</v>
+      </c>
+      <c r="E75" t="n">
+        <v>0.0470738410949707</v>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t xml:space="preserve">⎛ C ⎞⎛  ∅  ⎞
+⎝ ∅ ⎠⎝ a,b ⎠
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>011111</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>111111</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>Geometric</t>
+        </is>
+      </c>
+      <c r="D76" t="n">
+        <v>2.3125</v>
+      </c>
+      <c r="E76" t="n">
+        <v>0.0504150390625</v>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t xml:space="preserve">⎛ C ⎞⎛  ∅  ⎞
+⎝ ∅ ⎠⎝ a,b ⎠
 </t>
         </is>
       </c>

</xml_diff>

<commit_message>
tabla de costos lista para sacar particiones
</commit_message>
<xml_diff>
--- a/PruebasTaller2.xlsx
+++ b/PruebasTaller2.xlsx
@@ -1934,7 +1934,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F76"/>
+  <dimension ref="A1:F90"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3899,15 +3899,11 @@
       </c>
     </row>
     <row r="76">
-      <c r="A76" t="inlineStr">
-        <is>
-          <t>011111</t>
-        </is>
-      </c>
-      <c r="B76" t="inlineStr">
-        <is>
-          <t>111111</t>
-        </is>
+      <c r="A76" t="n">
+        <v>11111</v>
+      </c>
+      <c r="B76" t="n">
+        <v>111111</v>
       </c>
       <c r="C76" t="inlineStr">
         <is>
@@ -3924,6 +3920,374 @@
         <is>
           <t xml:space="preserve">⎛ C ⎞⎛  ∅  ⎞
 ⎝ ∅ ⎠⎝ a,b ⎠
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>11111</v>
+      </c>
+      <c r="B77" t="n">
+        <v>111111</v>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>Geometric</t>
+        </is>
+      </c>
+      <c r="D77" t="n">
+        <v>2.3125</v>
+      </c>
+      <c r="E77" t="n">
+        <v>0.0827491283416748</v>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t xml:space="preserve">⎛ C ⎞⎛  ∅  ⎞
+⎝ ∅ ⎠⎝ a,b ⎠
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>11111</v>
+      </c>
+      <c r="B78" t="n">
+        <v>111111</v>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>Geometric</t>
+        </is>
+      </c>
+      <c r="D78" t="n">
+        <v>2.3125</v>
+      </c>
+      <c r="E78" t="n">
+        <v>0.06886148452758789</v>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t xml:space="preserve">⎛ C ⎞⎛  ∅  ⎞
+⎝ ∅ ⎠⎝ a,b ⎠
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>111111111111111</v>
+      </c>
+      <c r="B79" t="n">
+        <v>111111111111111</v>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>Geometric</t>
+        </is>
+      </c>
+      <c r="D79" t="n">
+        <v>14.74831676483154</v>
+      </c>
+      <c r="E79" t="n">
+        <v>0.5017726421356201</v>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t xml:space="preserve">⎛ B ⎞⎛  ∅  ⎞
+⎝ ∅ ⎠⎝ a,c ⎠
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>111111111111111</v>
+      </c>
+      <c r="B80" t="n">
+        <v>111111111111110</v>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>Geometric</t>
+        </is>
+      </c>
+      <c r="D80" t="n">
+        <v>14.73581600189209</v>
+      </c>
+      <c r="E80" t="n">
+        <v>0.5791902542114258</v>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t xml:space="preserve">⎛ B ⎞⎛  ∅  ⎞
+⎝ ∅ ⎠⎝ a,c ⎠
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>111111111111111</v>
+      </c>
+      <c r="B81" t="n">
+        <v>111111111111110</v>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>Geometric</t>
+        </is>
+      </c>
+      <c r="D81" t="n">
+        <v>14.73581600189209</v>
+      </c>
+      <c r="E81" t="n">
+        <v>0.5802597999572754</v>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t xml:space="preserve">⎛ B ⎞⎛  ∅  ⎞
+⎝ ∅ ⎠⎝ a,c ⎠
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>111111111111111</v>
+      </c>
+      <c r="B82" t="n">
+        <v>111111111111110</v>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>Geometric</t>
+        </is>
+      </c>
+      <c r="D82" t="n">
+        <v>14.73581600189209</v>
+      </c>
+      <c r="E82" t="n">
+        <v>0.5879178047180176</v>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t xml:space="preserve">⎛ B ⎞⎛  ∅  ⎞
+⎝ ∅ ⎠⎝ a,c ⎠
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>111111111111111</v>
+      </c>
+      <c r="B83" t="n">
+        <v>111111111111110</v>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>Geometric</t>
+        </is>
+      </c>
+      <c r="D83" t="n">
+        <v>14.73581600189209</v>
+      </c>
+      <c r="E83" t="n">
+        <v>0.470977783203125</v>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t xml:space="preserve">⎛ B ⎞⎛  ∅  ⎞
+⎝ ∅ ⎠⎝ a,c ⎠
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>111111111111111</v>
+      </c>
+      <c r="B84" t="n">
+        <v>111111111111111</v>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>Geometric</t>
+        </is>
+      </c>
+      <c r="D84" t="n">
+        <v>14.74831676483154</v>
+      </c>
+      <c r="E84" t="n">
+        <v>0.4847466945648193</v>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t xml:space="preserve">⎛ B ⎞⎛  ∅  ⎞
+⎝ ∅ ⎠⎝ a,c ⎠
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>111111111111100</v>
+      </c>
+      <c r="B85" t="n">
+        <v>111111111111111</v>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>Geometric</t>
+        </is>
+      </c>
+      <c r="D85" t="n">
+        <v>12.77331638336182</v>
+      </c>
+      <c r="E85" t="n">
+        <v>0.5350770950317383</v>
+      </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t xml:space="preserve">⎛ B ⎞⎛  ∅  ⎞
+⎝ ∅ ⎠⎝ a,c ⎠
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>111111111000000</v>
+      </c>
+      <c r="B86" t="n">
+        <v>1111111111</v>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>Geometric</t>
+        </is>
+      </c>
+      <c r="D86" t="n">
+        <v>8.783961296081543</v>
+      </c>
+      <c r="E86" t="n">
+        <v>89.12561917304993</v>
+      </c>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t xml:space="preserve">⎛ B ⎞⎛  ∅  ⎞
+⎝ ∅ ⎠⎝ a,c ⎠
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>111111111111111</v>
+      </c>
+      <c r="B87" t="n">
+        <v>111111111111111</v>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>Geometric</t>
+        </is>
+      </c>
+      <c r="D87" t="n">
+        <v>14.74831676483154</v>
+      </c>
+      <c r="E87" t="n">
+        <v>0.4873776435852051</v>
+      </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t xml:space="preserve">⎛ B ⎞⎛  ∅  ⎞
+⎝ ∅ ⎠⎝ a,c ⎠
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>111111111111111</v>
+      </c>
+      <c r="B88" t="n">
+        <v>110110110110110</v>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>Geometric</t>
+        </is>
+      </c>
+      <c r="D88" t="n">
+        <v>14.61851978302002</v>
+      </c>
+      <c r="E88" t="n">
+        <v>1.16145920753479</v>
+      </c>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t xml:space="preserve">⎛ B ⎞⎛  ∅  ⎞
+⎝ ∅ ⎠⎝ a,c ⎠
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>111111111111111</v>
+      </c>
+      <c r="B89" t="n">
+        <v>111111111111111</v>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>Geometric</t>
+        </is>
+      </c>
+      <c r="D89" t="n">
+        <v>14.74831676483154</v>
+      </c>
+      <c r="E89" t="n">
+        <v>0.4490947723388672</v>
+      </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t xml:space="preserve">⎛ B ⎞⎛  ∅  ⎞
+⎝ ∅ ⎠⎝ a,c ⎠
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>111111111111111</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>110110110110110</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>Geometric</t>
+        </is>
+      </c>
+      <c r="D90" t="n">
+        <v>14.61851978302002</v>
+      </c>
+      <c r="E90" t="n">
+        <v>1.101146697998047</v>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t xml:space="preserve">⎛ B ⎞⎛  ∅  ⎞
+⎝ ∅ ⎠⎝ a,c ⎠
 </t>
         </is>
       </c>

</xml_diff>